<commit_message>
With .gitignore file to ignore screenshots folders
</commit_message>
<xml_diff>
--- a/WeeklyAmexCreditCardTransactions_GatherDaily/Data/Config.xlsx
+++ b/WeeklyAmexCreditCardTransactions_GatherDaily/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feb79f201121421/UiPATH/WeeklyAmexCreditCardTransactions_GatherDaily/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surya\OneDrive\UiPATH\WeeklyAmexCreditCardTransactions_GatherDaily\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{8FF4AB75-E890-4003-8F10-A5C473EDA49B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0795E231-205D-4F37-BE0F-EE5EA345D7C1}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{8FF4AB75-E890-4003-8F10-A5C473EDA49B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{39D7BD69-B547-4542-8955-9BEA9044370F}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="240" windowWidth="15375" windowHeight="8715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24645" yWindow="990" windowWidth="21615" windowHeight="8715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>CWD</t>
   </si>
   <si>
-    <t>WeeklyCreditCardTransactions_GatherDaily</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>https://online.americanexpress.com/myca/estmt/us/list.do?viewLegacyPage=Y&amp;BPIndex=0&amp;request_type=authreg_Statement&amp;inav=myca_statements&amp;Face=en_US&amp;sorted_index=0</t>
+  </si>
+  <si>
+    <t>WeeklyCitiCreditCardTransactions_GatherDaily</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -640,39 +640,39 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>